<commit_message>
se añade lectura de juicio general
</commit_message>
<xml_diff>
--- a/PRO_28112023A/Templates/template.xlsx
+++ b/PRO_28112023A/Templates/template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\5. Independiente\Proameise\28112023-A\PRO_28112023A\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\0. Trabajo\Proameise\PRO_28112023-A-AllenBradley\PRO_28112023A\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Date//time produced part</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t xml:space="preserve">Software of actuator </t>
+  </si>
+  <si>
+    <t>General Judge</t>
   </si>
 </sst>
 </file>
@@ -489,15 +492,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD13"/>
+      <selection activeCell="V2" sqref="V2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:20" s="1" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" s="1" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -546,8 +549,11 @@
       <c r="T1" s="4" t="s">
         <v>21</v>
       </c>
+      <c r="U1" s="4" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="2" spans="1:20" s="2" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" s="2" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -584,9 +590,11 @@
       <c r="R2" s="4"/>
       <c r="S2" s="4"/>
       <c r="T2" s="4"/>
+      <c r="U2" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="15">
+    <mergeCell ref="U1:U2"/>
     <mergeCell ref="T1:T2"/>
     <mergeCell ref="P1:P2"/>
     <mergeCell ref="M1:M2"/>

</xml_diff>